<commit_message>
- adjustments made to finish by 20th - elaborated milestones for code completion, documentation and test demonstration - added 2 new columns for checking completion of milestone and mark obtained
</commit_message>
<xml_diff>
--- a/kdea020-medsci736-milestones.xlsx
+++ b/kdea020-medsci736-milestones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Milestone</t>
   </si>
@@ -44,22 +44,31 @@
     <t xml:space="preserve">TDD check </t>
   </si>
   <si>
-    <t>Modularisation complete</t>
-  </si>
-  <si>
     <t>Potentially shippable (code to Sanjid, he can run and use)</t>
   </si>
   <si>
-    <t>Code completion check</t>
-  </si>
-  <si>
-    <t>Documentation finalised</t>
-  </si>
-  <si>
     <t>Code finalised</t>
   </si>
   <si>
-    <t>Demonstration – All tests should pass</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Demonstration of the product</t>
+  </si>
+  <si>
+    <t>Documentation finalised (including RM, metadata &amp;  License)</t>
+  </si>
+  <si>
+    <t>Code completion check (consistent with Trello Board)</t>
+  </si>
+  <si>
+    <t>Modularisation complete (ogranised directory and functions)</t>
+  </si>
+  <si>
+    <t>All tests must be complete and pass (consistent with Trello Board)</t>
+  </si>
+  <si>
+    <t>Obtained</t>
   </si>
 </sst>
 </file>
@@ -69,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,6 +88,22 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -101,8 +126,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -110,7 +143,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,20 +481,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +504,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -474,8 +521,14 @@
       <c r="C2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -485,8 +538,14 @@
       <c r="C3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -496,8 +555,14 @@
       <c r="C4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -507,8 +572,14 @@
       <c r="C5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -518,21 +589,33 @@
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>42649</v>
+        <v>42652</v>
       </c>
       <c r="C7" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>42656</v>
@@ -541,7 +624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -552,9 +635,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>42661</v>
@@ -563,9 +646,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>42661</v>
@@ -574,40 +657,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
-        <v>42663</v>
+        <v>42661</v>
       </c>
       <c r="C12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3">
         <v>42663</v>
       </c>
       <c r="C13" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2">
-        <v>42668</v>
+        <v>42663</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5">
       <c r="C15" s="1">
         <f>SUM(C2:C14)</f>
         <v>100</v>
@@ -615,7 +698,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>